<commit_message>
project and notes added
</commit_message>
<xml_diff>
--- a/Excel/Excel Final project data.xlsx
+++ b/Excel/Excel Final project data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishan\Desktop\Bootcamp.Info\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E83009-A785-475A-B0B0-A7FEA154F1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730F9B76-E13F-4198-805A-2FB521A4CBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,17 +18,18 @@
     <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet6" sheetId="7" r:id="rId5"/>
-    <sheet name="heart_failure_clinical_records_" sheetId="1" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId6"/>
+    <sheet name="heart_failure_clinical_records_" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="59" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="35">
   <si>
     <t>age</t>
   </si>
@@ -127,9 +128,6 @@
   </si>
   <si>
     <t>Average of anaemia</t>
-  </si>
-  <si>
-    <t>Count of DEATH_EVENT</t>
   </si>
   <si>
     <t>Average of diabetes</t>
@@ -701,10 +699,136 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Excel Final project data.xlsx]Sheet5!PivotTable44</c:name>
-    <c:fmtId val="61"/>
+    <c:name>[Excel Final project data.xlsx]Sheet3!PivotTable1</c:name>
+    <c:fmtId val="4"/>
   </c:pivotSource>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Positive Smoking History: Death Vs Survival</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16072222222222221"/>
+          <c:y val="0.11943260393354235"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
@@ -752,9 +876,8 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -766,6 +889,62 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -825,7 +1004,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -833,11 +1012,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$B$3</c:f>
+              <c:f>Sheet3!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average of serum_sodium</c:v>
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -911,160 +1090,59 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet5!$A$4:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Died</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Survived</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(blank)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet3!$A$4:$A$10</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Female</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Male</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Female</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Male</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Died</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Survived</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$B$4:$B$7</c:f>
+              <c:f>Sheet3!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>135.375</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>137.21674876847291</c:v>
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D18D-4FF0-B49B-98E031B447EB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet5!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Count of DEATH_EVENT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet5!$A$4:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Died</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Survived</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(blank)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet5!$C$4:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>203</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D18D-4FF0-B49B-98E031B447EB}"/>
+              <c16:uniqueId val="{00000003-D11D-473F-90F2-C50780528EB6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1077,18 +1155,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="539235704"/>
-        <c:axId val="539231768"/>
+        <c:gapWidth val="182"/>
+        <c:axId val="534001200"/>
+        <c:axId val="533998904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539235704"/>
+        <c:axId val="534001200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1126,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539231768"/>
+        <c:crossAx val="533998904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1134,12 +1211,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539231768"/>
+        <c:axId val="533998904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1185,7 +1262,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539235704"/>
+        <c:crossAx val="534001200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1197,37 +1274,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1275,7 +1321,6 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -1329,7 +1374,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1533,22 +1578,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1653,8 +1699,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1786,19 +1832,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1835,23 +1882,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AB4FA65-3EA0-44EB-9564-3DA622C92B01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B439E0FD-4618-419E-9D3B-69FF24B10676}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6493,8 +6540,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E93EE73D-16F2-4D2C-A308-2D0B8CC44504}" name="PivotTable1" cacheId="59" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A3:H12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E93EE73D-16F2-4D2C-A308-2D0B8CC44504}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:H11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -6519,7 +6566,7 @@
       <items count="4">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
+        <item sd="0" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6528,7 +6575,7 @@
     <field x="12"/>
     <field x="9"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="8">
     <i>
       <x/>
     </i>
@@ -6548,9 +6595,6 @@
       <x v="1"/>
     </i>
     <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
       <x v="2"/>
     </i>
     <i t="grand">
@@ -6605,8 +6649,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CAF2D820-0D67-45EC-A9CD-52E1ABDBF213}" name="PivotTable1" cacheId="59" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CAF2D820-0D67-45EC-A9CD-52E1ABDBF213}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0">
       <items count="49">
@@ -6683,7 +6727,7 @@
       <items count="4">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
+        <item n=" " h="1" sd="0" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6692,7 +6736,7 @@
     <field x="12"/>
     <field x="9"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -6710,12 +6754,6 @@
     </i>
     <i r="1">
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -6740,7 +6778,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D192C127-B8C2-4E78-A830-29C8140F993A}" name="PivotTable3" cacheId="59" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D192C127-B8C2-4E78-A830-29C8140F993A}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:E12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -6840,146 +6878,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DD5A3A08-058D-46FF-AEFC-5F140BA19AD0}" name="PivotTable44" cacheId="59" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="65">
-  <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="12"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Average of serum_sodium" fld="8" subtotal="average" baseField="12" baseItem="0"/>
-    <dataField name="Count of DEATH_EVENT" fld="12" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="6">
-    <chartFormat chart="32" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="29" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="61" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="61" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="32" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="30" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{199E80AE-9353-4D2C-B586-4C984A6BE9E6}" name="PivotTable45" cacheId="59" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{199E80AE-9353-4D2C-B586-4C984A6BE9E6}" name="PivotTable45" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:L12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField dataField="1" showAll="0"/>
@@ -7094,6 +6993,103 @@
     <dataField name="Average of smoking" fld="10" subtotal="average" baseField="12" baseItem="0"/>
     <dataField name="Average of ejection_fraction" fld="4" subtotal="average" baseField="12" baseItem="0"/>
   </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{041D4B1C-80B4-40A7-9B6B-6D71C9798336}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="12"/>
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of smoking" fld="10" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="4" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -7403,10 +7399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD50DFE-0428-43D7-A7BF-FF8FA1D31BD2}">
-  <dimension ref="A3:H12"/>
+  <dimension ref="A3:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7633,40 +7629,28 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B11" s="4">
         <v>299</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C11" s="4">
         <v>60.833892976588636</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D11" s="4">
         <v>129</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E11" s="4">
         <v>125</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F11" s="4">
         <v>105</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G11" s="4">
         <v>96</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H11" s="4">
         <v>38.083612040133779</v>
       </c>
     </row>
@@ -7677,10 +7661,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8745C152-FEAA-4EB4-9461-30081E859C4D}">
-  <dimension ref="A3:B12"/>
+  <dimension ref="A3:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7747,21 +7731,9 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B10" s="4">
         <v>581.83946488294316</v>
       </c>
     </row>
@@ -7775,7 +7747,7 @@
   <dimension ref="A3:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7948,78 +7920,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF92CBB7-5922-4F3B-A7C2-E69999AA2FBB}">
-  <dimension ref="A3:C7"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A3:B7"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4">
-        <v>135.375</v>
-      </c>
-      <c r="C4" s="4">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="4">
-        <v>137.21674876847291</v>
-      </c>
-      <c r="C5" s="4">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="4">
-        <v>136.62541806020067</v>
-      </c>
-      <c r="C7" s="4">
-        <v>299</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8027,7 +7947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E233C8-4059-4850-ACAD-A3C252961AF3}">
   <dimension ref="A2:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="A3:L12"/>
     </sheetView>
   </sheetViews>
@@ -8074,13 +7994,13 @@
         <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
         <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
         <v>25</v>
@@ -8390,6 +8310,90 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEBD8C6-E15E-4DF6-8034-226C62745EE8}">
+  <dimension ref="A3:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M300"/>
   <sheetViews>

</xml_diff>